<commit_message>
Updated Annadata Sukhibhava expenditure data in cleaned Excel with FY2025-26 BE
</commit_message>
<xml_diff>
--- a/Documentation/data_acquisition_log.xlsx
+++ b/Documentation/data_acquisition_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_AP_Welfare_Dashboard\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA611BA4-F244-4D42-B2DA-86DD6F6D9FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C7A19F-4B0B-47F5-88CA-D1D3A1224EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Source_Name</t>
   </si>
@@ -67,6 +67,18 @@
   </si>
   <si>
     <t>"C:\Project_AP_Welfare_Dashboard\Data\Raw\APFinance24-25Vol1.pdf"</t>
+  </si>
+  <si>
+    <t>https://apfinance.gov.in/...Bud@et24-25/documents/Volume-III-11.pdf</t>
+  </si>
+  <si>
+    <t>Agriculture &amp; Co-Operation &amp; Food, Civil Supplies &amp; Consumers Affairs Department</t>
+  </si>
+  <si>
+    <t>Scheme-wise data for Annadata Sukhibhava (current farmer scheme) and Vaddi Leni Runalu (VLR) found in 'LIST OF SCHEMES' table starting on Page 67. All figures are in Rupees Lakhs. YSR Rythu Bharosa was the previous scheme, Annadata Sukhibhava is the current one</t>
+  </si>
+  <si>
+    <t>"C:\Project_AP_Welfare_Dashboard\Data\Raw\Agriculture_data.pdf"</t>
   </si>
 </sst>
 </file>
@@ -132,12 +144,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -149,6 +161,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -430,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,7 +463,7 @@
     <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.88671875" customWidth="1"/>
     <col min="8" max="8" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -498,10 +517,38 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="10">
+        <v>45845</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{7377D159-1BC9-4813-B284-1680866812D4}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{3A3991D9-B0D4-458E-A44A-4FFD8D15EC1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated data acquisition log with all downloaded budget documents and G.O.
</commit_message>
<xml_diff>
--- a/Documentation/data_acquisition_log.xlsx
+++ b/Documentation/data_acquisition_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project_AP_Welfare_Dashboard\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C7A19F-4B0B-47F5-88CA-D1D3A1224EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE49ACC-756A-4620-A33A-955C4CBB55C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Source_Name</t>
   </si>
@@ -79,13 +79,43 @@
   </si>
   <si>
     <t>"C:\Project_AP_Welfare_Dashboard\Data\Raw\Agriculture_data.pdf"</t>
+  </si>
+  <si>
+    <t>https://apfinance.gov.in/...Bud@et25-26/documents/Volume-III-14.pdf</t>
+  </si>
+  <si>
+    <t>https://apfinance.gov.in/...Bud@et24-25/documents/Volume-III-14.pdf</t>
+  </si>
+  <si>
+    <t>2025-26</t>
+  </si>
+  <si>
+    <t>2024-25 RD Data</t>
+  </si>
+  <si>
+    <t>2025-26 RD Data</t>
+  </si>
+  <si>
+    <t>PANCHAYAT RAJ AND RURAL DEVELOPMENT (RD.I) DEPARTMENT</t>
+  </si>
+  <si>
+    <t>New_Pension_scheme</t>
+  </si>
+  <si>
+    <t>C:\Project_AP_Welfare_Dashboard\Data\Raw\New_Pensions_Scheme.pdf</t>
+  </si>
+  <si>
+    <t>C:\Project_AP_Welfare_Dashboard\Data\Raw\2025-26 RD Data.pdf</t>
+  </si>
+  <si>
+    <t>C:\Project_AP_Welfare_Dashboard\Data\Raw\2024-25 RD Data.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +127,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,7 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -161,13 +197,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -449,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G6" sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,38 +546,111 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="7">
+        <v>45845</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="7">
         <v>45845</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
+      <c r="G4" s="4"/>
+      <c r="H4" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7">
+        <v>45845</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="7">
+        <v>45845</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{7377D159-1BC9-4813-B284-1680866812D4}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{3A3991D9-B0D4-458E-A44A-4FFD8D15EC1E}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{3A3991D9-B0D4-458E-A44A-4FFD8D15EC1E}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{E0636BC3-4AEA-4A39-9F1F-A8E75DC3DB12}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{728607C9-A20D-4272-B2FA-FE01872AD5F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>